<commit_message>
Added time taken to complete tasks
</commit_message>
<xml_diff>
--- a/Study Participant Data.xlsx
+++ b/Study Participant Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pesek\SoftEngineering\SoftSpring2025\RegexStudy\Eye-Tracking-Study-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054EE26D-5A27-4177-B572-6F9B119F5DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C485AA00-2277-4866-808F-02F4630079BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="17385" activeTab="1" xr2:uid="{79C6930F-352E-4A49-9B6B-B85534897C81}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
   <si>
     <t>ID Number</t>
   </si>
@@ -142,12 +142,27 @@
   </si>
   <si>
     <t>Correct</t>
+  </si>
+  <si>
+    <t>Task 1 Time</t>
+  </si>
+  <si>
+    <t>Task 2 Time</t>
+  </si>
+  <si>
+    <t>Task 3 Time</t>
+  </si>
+  <si>
+    <t>Task 4 Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="h:mm;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,9 +192,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,7 +533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA11650D-922A-40C9-8877-59A4DABC015C}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
@@ -843,10 +860,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E01B001A-7B75-471B-B47D-99F66C1162A0}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,9 +872,10 @@
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -873,8 +891,20 @@
       <c r="E1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -890,8 +920,20 @@
       <c r="E2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="3">
+        <v>9.375E-2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>0.19930555555555557</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="I2" s="2">
+        <v>0.49305555555555558</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -907,8 +949,20 @@
       <c r="E3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <v>0.1125</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.2388888888888889</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0.22430555555555556</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.22638888888888889</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -924,8 +978,20 @@
       <c r="E4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="2">
+        <v>0.15763888888888888</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.20624999999999999</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.30972222222222223</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.26111111111111113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -941,8 +1007,20 @@
       <c r="E5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="2">
+        <v>0.21319444444444444</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0.28194444444444444</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.29097222222222224</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.3034722222222222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -958,8 +1036,20 @@
       <c r="E6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="2">
+        <v>0.12291666666666666</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.14305555555555555</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.15625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -975,8 +1065,20 @@
       <c r="E7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="2">
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.15763888888888888</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.19722222222222222</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.25833333333333336</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -991,6 +1093,18 @@
       </c>
       <c r="E8" t="s">
         <v>33</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.10486111111111111</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.11180555555555556</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.15069444444444444</v>
+      </c>
+      <c r="I8" s="2">
+        <v>8.3333333333333329E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>